<commit_message>
measure diameter for normal temperature
</commit_message>
<xml_diff>
--- a/kiwi_data.xlsx
+++ b/kiwi_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D03A16A-6B54-4C88-A045-F1B713A51E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A409FC6-6D44-47CA-93CB-4DFCCFEA7019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="冷库" sheetId="1" r:id="rId1"/>
@@ -1212,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1476,7 @@
         <v>50.19</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>47.27</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>48.29</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>47.38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -1508,15 +1508,18 @@
         <v>46.79</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37">
         <v>45.83</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>46.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>49.13</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>48.79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1540,476 +1543,653 @@
         <v>47.78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
       <c r="B41">
         <v>48.52</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>47.91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
       <c r="B42">
         <v>44.19</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>43.89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
       <c r="B43">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>43.86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
       <c r="B44">
         <v>50.19</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>47.91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
       <c r="B45">
         <v>43.95</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>43.23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
       <c r="B46">
         <v>46.52</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>45.97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
       <c r="B47">
         <v>50.53</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>49.55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
       <c r="B48">
         <v>50.98</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
       <c r="B49">
         <v>50.96</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>49.74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
       <c r="B50">
         <v>43.43</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>42.17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
       <c r="B51">
         <v>48.87</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>47.97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
       <c r="B52">
         <v>49.85</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>49.67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
       <c r="B53">
         <v>45.73</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>45.96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
       <c r="B54">
         <v>48.61</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>47.78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
       <c r="B55">
         <v>47.53</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>47.17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
       <c r="B56">
         <v>46.56</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>45.53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
       <c r="B57">
         <v>48.57</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>47.23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
       <c r="B58">
         <v>47.14</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>46.65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
       <c r="B59">
         <v>42.58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>42.71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>60</v>
       </c>
       <c r="B60">
         <v>47.05</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>46.56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
       <c r="B61">
         <v>49.77</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>48.09</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
       <c r="B62">
         <v>47.84</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>47.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
       <c r="B63">
         <v>48.96</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>48.41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
       </c>
       <c r="B64">
         <v>47.06</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>46.63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>65</v>
       </c>
       <c r="B65">
         <v>42.93</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>42.06</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>66</v>
       </c>
       <c r="B66">
         <v>46.05</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>45.49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
       <c r="B67">
         <v>46.35</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>46.29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
       <c r="B68">
         <v>50.54</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>49.71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
       <c r="B69">
         <v>48.52</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>47.05</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
       <c r="B70">
         <v>44.93</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>44.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>71</v>
       </c>
       <c r="B71">
         <v>46.07</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>45.12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>72</v>
       </c>
       <c r="B72">
         <v>48.95</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>48.34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
       <c r="B73">
         <v>46.77</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>47.09</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>74</v>
       </c>
       <c r="B74">
         <v>50.3</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>50.05</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>75</v>
       </c>
       <c r="B75">
         <v>49.95</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>49.44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>76</v>
       </c>
       <c r="B76">
         <v>48.21</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>48.61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>77</v>
       </c>
       <c r="B77">
         <v>48.08</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>47.83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>78</v>
       </c>
       <c r="B78">
         <v>50.03</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>50.06</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>79</v>
       </c>
       <c r="B79">
         <v>46.47</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>46.04</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>80</v>
       </c>
       <c r="B80">
         <v>46.81</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>45.77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>81</v>
       </c>
       <c r="B81">
         <v>49.34</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>49.06</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>82</v>
       </c>
       <c r="B82">
         <v>48.12</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>83</v>
       </c>
       <c r="B83">
         <v>48.19</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>47.17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>84</v>
       </c>
       <c r="B84">
         <v>48.85</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>48.06</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>85</v>
       </c>
       <c r="B85">
         <v>49.62</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>48.48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>86</v>
       </c>
       <c r="B86">
         <v>48.43</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>48.11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>87</v>
       </c>
       <c r="B87">
         <v>51.12</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>88</v>
       </c>
       <c r="B88">
         <v>48.39</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>48.83</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>89</v>
       </c>
       <c r="B89">
         <v>50.06</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>49.26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90</v>
       </c>
       <c r="B90">
         <v>48.85</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>48.42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>91</v>
       </c>
       <c r="B91">
         <v>45.62</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>45.38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
       <c r="B92">
         <v>51.14</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>49.56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>93</v>
       </c>
       <c r="B93">
         <v>45.48</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>44.59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>94</v>
       </c>
       <c r="B94">
         <v>48.52</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>47.59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>95</v>
       </c>
       <c r="B95">
         <v>46.31</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>45.41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>96</v>
       </c>
       <c r="B96">
         <v>50.94</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>50.35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>97</v>
       </c>
       <c r="B97">
         <v>47.94</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>47.26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>98</v>
       </c>
       <c r="B98">
         <v>48.32</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>47.23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>99</v>
       </c>
       <c r="B99">
         <v>52.78</v>
+      </c>
+      <c r="C99">
+        <v>51.67</v>
       </c>
     </row>
   </sheetData>
@@ -2156,7 +2336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>

</xml_diff>